<commit_message>
updates list of supported fuml concepts
</commit_message>
<xml_diff>
--- a/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
+++ b/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Syntax!$A$1:$B$125</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="135">
   <si>
     <t>Actions</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>Class Diagrams</t>
+  </si>
+  <si>
+    <t>partly</t>
+  </si>
+  <si>
+    <t>defining an activity as decision node input behavior is not supported</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +461,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -520,6 +538,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -814,9 +842,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -1024,20 +1054,20 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="D13" s="23"/>
+      <c r="E13" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1054,38 +1084,38 @@
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="D16" s="20"/>
+      <c r="E16" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1108,75 +1138,75 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="A19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>129</v>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>129</v>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="11" customFormat="1">
@@ -1574,38 +1604,38 @@
       <c r="F44" s="12"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F45" s="4" t="s">
+      <c r="D45" s="23"/>
+      <c r="E45" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F45" s="24" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" s="4" t="s">
+      <c r="D46" s="23"/>
+      <c r="E46" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" s="24" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1628,42 +1658,42 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="1" t="s">
+      <c r="D48" s="23"/>
+      <c r="E48" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="11" customFormat="1">
+      <c r="D49" s="23"/>
+      <c r="E49" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="11" customFormat="1">
       <c r="A50" s="8" t="s">
         <v>4</v>
       </c>
@@ -1675,7 +1705,7 @@
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -1693,7 +1723,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
         <v>4</v>
       </c>
@@ -1711,7 +1741,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1759,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="11" customFormat="1">
+    <row r="54" spans="1:7" s="11" customFormat="1">
       <c r="A54" s="8" t="s">
         <v>4</v>
       </c>
@@ -1741,7 +1771,7 @@
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
         <v>4</v>
       </c>
@@ -1759,7 +1789,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
         <v>4</v>
       </c>
@@ -1777,7 +1807,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -1795,7 +1825,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
@@ -1813,7 +1843,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
@@ -1831,7 +1861,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
         <v>4</v>
       </c>
@@ -1849,7 +1879,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
         <v>4</v>
       </c>
@@ -1867,7 +1897,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
         <v>4</v>
       </c>
@@ -1882,10 +1912,13 @@
         <v>127</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>133</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
         <v>4</v>
       </c>
@@ -1903,7 +1936,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
adds test case for read extent action
</commit_message>
<xml_diff>
--- a/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
+++ b/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19440" windowHeight="10560"/>
   </bookViews>
   <sheets>
     <sheet name="Syntax" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Syntax!$A$1:$B$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Syntax!$A$1:$B$129</definedName>
   </definedNames>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="140">
   <si>
     <t>Actions</t>
   </si>
@@ -422,6 +422,21 @@
   </si>
   <si>
     <t>defining an activity as decision node input behavior is not supported</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>actions with isLocallyReentrant = true are not supported</t>
+  </si>
+  <si>
+    <t>mustIsolate = true has no effect</t>
+  </si>
+  <si>
+    <t>no difference between mode iterative and mode parallel implemented</t>
+  </si>
+  <si>
+    <t>only support primitive behaviors</t>
   </si>
 </sst>
 </file>
@@ -445,7 +460,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,24 +475,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -500,11 +509,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -533,20 +662,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -856,140 +1023,127 @@
     <col min="4" max="4" width="63.140625" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="5"/>
+    <col min="7" max="7" width="65.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1">
-      <c r="A2" s="16" t="s">
+      <c r="G1" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1">
+      <c r="A3" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:6" s="11" customFormat="1">
-      <c r="A3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" s="11" customFormat="1">
-      <c r="A4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" s="11" customFormat="1">
+      <c r="A5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" s="11" customFormat="1">
+      <c r="A6" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C7" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
@@ -998,34 +1152,36 @@
       <c r="F9" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
+      <c r="G9" s="29"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
@@ -1034,16 +1190,17 @@
       <c r="F11" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
@@ -1052,220 +1209,235 @@
       <c r="F12" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="22" t="s">
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="11" customFormat="1">
-      <c r="A14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="D15" s="17"/>
+      <c r="E15" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" s="11" customFormat="1">
+      <c r="A16" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="22" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="19" t="s">
+      <c r="D17" s="17"/>
+      <c r="E17" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="37"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C18" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="D18" s="46"/>
+      <c r="E18" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="48"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="19" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="19" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="43"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="22" t="s">
+      <c r="D21" s="17"/>
+      <c r="E21" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="22" t="s">
+      <c r="D22" s="17"/>
+      <c r="E22" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="37"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C23" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="11" customFormat="1">
-      <c r="A22" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="D23" s="17"/>
+      <c r="E23" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="37"/>
+    </row>
+    <row r="24" spans="1:7" s="11" customFormat="1">
+      <c r="A24" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="27"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="4" t="s">
@@ -1274,16 +1446,17 @@
       <c r="F25" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
+      <c r="G25" s="29"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="4" t="s">
@@ -1292,16 +1465,17 @@
       <c r="F26" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
+      <c r="G26" s="29"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="4" t="s">
@@ -1310,16 +1484,17 @@
       <c r="F27" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1" t="s">
+      <c r="G27" s="29"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="4" t="s">
@@ -1328,16 +1503,17 @@
       <c r="F28" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="1" t="s">
+      <c r="G28" s="29"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="4" t="s">
@@ -1346,34 +1522,36 @@
       <c r="F29" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1" t="s">
+      <c r="G29" s="29"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
+      <c r="G30" s="29"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="4" t="s">
@@ -1382,34 +1560,36 @@
       <c r="F31" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
+      <c r="G31" s="29"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="1" t="s">
+      <c r="G32" s="29"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="4" t="s">
@@ -1418,16 +1598,17 @@
       <c r="F33" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="1" t="s">
+      <c r="G33" s="29"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="4" t="s">
@@ -1436,16 +1617,17 @@
       <c r="F34" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1" t="s">
+      <c r="G34" s="29"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="4" t="s">
@@ -1454,16 +1636,17 @@
       <c r="F35" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1" t="s">
+      <c r="G35" s="29"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="4" t="s">
@@ -1472,16 +1655,17 @@
       <c r="F36" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1" t="s">
+      <c r="G36" s="29"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="4" t="s">
@@ -1490,34 +1674,36 @@
       <c r="F37" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="1" t="s">
+      <c r="G37" s="29"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1" t="s">
+      <c r="G38" s="29"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="4" t="s">
@@ -1526,230 +1712,246 @@
       <c r="F39" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="1" t="s">
+      <c r="G39" s="29"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" s="29"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="1" t="s">
+      <c r="G41" s="29"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="11" customFormat="1">
-      <c r="A43" s="8" t="s">
+      <c r="F42" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G42" s="29"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G44" s="29"/>
+    </row>
+    <row r="45" spans="1:7" s="11" customFormat="1">
+      <c r="A45" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="1:6" s="11" customFormat="1">
-      <c r="A44" s="8" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="27"/>
+    </row>
+    <row r="46" spans="1:7" s="11" customFormat="1">
+      <c r="A46" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="22" t="s">
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="27"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B47" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C47" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F45" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="22" t="s">
+      <c r="D47" s="17"/>
+      <c r="E47" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G47" s="37"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B48" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C48" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="1" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G48" s="37"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="22" t="s">
+      <c r="D49" s="2"/>
+      <c r="E49" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G49" s="29"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B50" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C50" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="22" t="s">
+      <c r="D50" s="17"/>
+      <c r="E50" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G50" s="37"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B51" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C51" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F49" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="11" customFormat="1">
-      <c r="A50" s="8" t="s">
+      <c r="D51" s="17"/>
+      <c r="E51" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="11" customFormat="1">
+      <c r="A52" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B52" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>125</v>
-      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="27"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="4" t="s">
@@ -1758,64 +1960,70 @@
       <c r="F53" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" s="11" customFormat="1">
-      <c r="A54" s="8" t="s">
+      <c r="G53" s="29"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="29"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="40"/>
+      <c r="E55" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F55" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="11" customFormat="1">
+      <c r="A56" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F55" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F56" s="13" t="s">
-        <v>125</v>
-      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="27"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="4" t="s">
@@ -1824,16 +2032,17 @@
       <c r="F57" s="13" t="s">
         <v>125</v>
       </c>
+      <c r="G57" s="29"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="4" t="s">
@@ -1842,16 +2051,17 @@
       <c r="F58" s="13" t="s">
         <v>125</v>
       </c>
+      <c r="G58" s="29"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="4" t="s">
@@ -1860,73 +2070,74 @@
       <c r="F59" s="13" t="s">
         <v>125</v>
       </c>
+      <c r="G59" s="29"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F60" s="13" t="s">
         <v>125</v>
       </c>
+      <c r="G60" s="29"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F61" s="13" t="s">
         <v>125</v>
       </c>
+      <c r="G61" s="29"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>134</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G62" s="29"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="4" t="s">
@@ -1935,52 +2146,57 @@
       <c r="F63" s="13" t="s">
         <v>125</v>
       </c>
+      <c r="G63" s="29"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F64" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="1" t="s">
+      <c r="C64" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64" s="40"/>
+      <c r="E64" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F64" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="G64" s="42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="1" t="s">
+      <c r="G65" s="29"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="4" t="s">
@@ -1989,16 +2205,17 @@
       <c r="F66" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="1" t="s">
+      <c r="G66" s="29"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="4" t="s">
@@ -2007,16 +2224,17 @@
       <c r="F67" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="1" t="s">
+      <c r="G67" s="29"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="4" t="s">
@@ -2025,917 +2243,1024 @@
       <c r="F68" s="13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="1" t="s">
+      <c r="G68" s="29"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G69" s="29"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G70" s="29"/>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A71" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="33"/>
+      <c r="E71" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="F71" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="G71" s="35"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="1:6" s="11" customFormat="1">
-      <c r="A71" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-    </row>
-    <row r="72" spans="1:6" s="11" customFormat="1">
-      <c r="A72" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="2" t="s">
+      <c r="B73" s="11"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A74" s="19"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" spans="1:7" s="11" customFormat="1">
+      <c r="A75" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="25"/>
+    </row>
+    <row r="76" spans="1:7" s="11" customFormat="1">
+      <c r="A76" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="27"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F73" s="4"/>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F74" s="14"/>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F75" s="13"/>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F76" s="14"/>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F77" s="13"/>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F77" s="4"/>
+      <c r="G77" s="29"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F78" s="13"/>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="1" t="s">
+      <c r="F78" s="14"/>
+      <c r="G78" s="29"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F79" s="13"/>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="1" t="s">
+      <c r="G79" s="29"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F80" s="13"/>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="1" t="s">
+      <c r="F80" s="14"/>
+      <c r="G80" s="29"/>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F81" s="13"/>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="1" t="s">
+      <c r="G81" s="29"/>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F82" s="13"/>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="1" t="s">
+      <c r="G82" s="29"/>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F83" s="13"/>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="1" t="s">
+      <c r="G83" s="29"/>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F84" s="14"/>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F84" s="13"/>
+      <c r="G84" s="29"/>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F85" s="13"/>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" s="1" t="s">
+      <c r="G85" s="29"/>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F86" s="13"/>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="1" t="s">
+      <c r="G86" s="29"/>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F87" s="13"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="1" t="s">
+      <c r="G87" s="29"/>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F88" s="14"/>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="1" t="s">
+      <c r="G88" s="29"/>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F89" s="13"/>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="1" t="s">
+      <c r="G89" s="29"/>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F90" s="14"/>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="1" t="s">
+      <c r="F90" s="13"/>
+      <c r="G90" s="29"/>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F91" s="13"/>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="1" t="s">
+      <c r="G91" s="29"/>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F92" s="13"/>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="1" t="s">
+      <c r="F92" s="14"/>
+      <c r="G92" s="29"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F93" s="14"/>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="1" t="s">
+      <c r="F93" s="13"/>
+      <c r="G93" s="29"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F94" s="13"/>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="1" t="s">
+      <c r="F94" s="14"/>
+      <c r="G94" s="29"/>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="4" t="s">
         <v>125</v>
       </c>
       <c r="F95" s="13"/>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="1" t="s">
+      <c r="G95" s="29"/>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F96" s="13"/>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="1" t="s">
+      <c r="G96" s="29"/>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F97" s="13"/>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="1" t="s">
+      <c r="F97" s="14"/>
+      <c r="G97" s="29"/>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F98" s="13"/>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="1" t="s">
+      <c r="G98" s="29"/>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="4" t="s">
         <v>125</v>
       </c>
       <c r="F99" s="13"/>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="1" t="s">
+      <c r="G99" s="29"/>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F100" s="13"/>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="1" t="s">
+      <c r="G100" s="29"/>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F101" s="13"/>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="1" t="s">
+      <c r="G101" s="29"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F102" s="13"/>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="1" t="s">
+      <c r="G102" s="29"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F103" s="13"/>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104" s="1" t="s">
+      <c r="G103" s="29"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F104" s="14"/>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105" s="1" t="s">
+      <c r="F104" s="13"/>
+      <c r="G104" s="29"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F105" s="13"/>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106" s="1" t="s">
+      <c r="G105" s="29"/>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F106" s="13"/>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="1" t="s">
+      <c r="G106" s="29"/>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F107" s="14"/>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F107" s="13"/>
+      <c r="G107" s="29"/>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D108" s="2"/>
       <c r="E108" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F108" s="14"/>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" s="1" t="s">
+      <c r="G108" s="29"/>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F109" s="13"/>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="1" t="s">
+      <c r="G109" s="29"/>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F110" s="13"/>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="1" t="s">
+      <c r="G110" s="29"/>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F111" s="14"/>
-    </row>
-    <row r="112" spans="1:6" s="11" customFormat="1">
-      <c r="A112" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="9"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
-    </row>
-    <row r="113" spans="1:6" s="11" customFormat="1">
-      <c r="A113" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C113" s="8"/>
-      <c r="D113" s="9"/>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="1" t="s">
-        <v>10</v>
+      <c r="G111" s="29"/>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F112" s="14"/>
+      <c r="G112" s="29"/>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F113" s="13"/>
+      <c r="G113" s="29"/>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="4" t="s">
         <v>125</v>
       </c>
       <c r="F114" s="13"/>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115" s="1" t="s">
-        <v>10</v>
+      <c r="G114" s="29"/>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D115" s="2"/>
       <c r="E115" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F115" s="13"/>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F115" s="14"/>
+      <c r="G115" s="29"/>
+    </row>
+    <row r="116" spans="1:7" s="11" customFormat="1">
+      <c r="A116" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="8"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+      <c r="G116" s="27"/>
+    </row>
+    <row r="117" spans="1:7" s="11" customFormat="1">
+      <c r="A117" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D116" s="2"/>
-      <c r="E116" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F116" s="13"/>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D117" s="2"/>
-      <c r="E117" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F117" s="13"/>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" s="1" t="s">
+      <c r="C117" s="8"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+      <c r="G117" s="27"/>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>117</v>
+      <c r="C118" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="D118" s="2"/>
       <c r="E118" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F118" s="13"/>
-    </row>
-    <row r="119" spans="1:6" s="11" customFormat="1">
-      <c r="A119" s="8" t="s">
+      <c r="G118" s="29"/>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C119" s="8"/>
-      <c r="D119" s="9"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" s="7" t="s">
+      <c r="B119" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F119" s="13"/>
+      <c r="G119" s="29"/>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D120" s="3"/>
-      <c r="E120" s="13" t="s">
-        <v>125</v>
+      <c r="B120" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D120" s="2"/>
+      <c r="E120" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="F120" s="13"/>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" s="1" t="s">
+      <c r="G120" s="29"/>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F121" s="4"/>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F121" s="13"/>
+      <c r="G121" s="29"/>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>120</v>
+        <v>11</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F122" s="4"/>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" s="1" t="s">
+      <c r="F122" s="13"/>
+      <c r="G122" s="29"/>
+    </row>
+    <row r="123" spans="1:7" s="11" customFormat="1">
+      <c r="A123" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D123" s="2"/>
-      <c r="E123" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F123" s="4"/>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="1" t="s">
+      <c r="C123" s="8"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+      <c r="G123" s="27"/>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D124" s="2"/>
-      <c r="E124" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F124" s="4"/>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="1" t="s">
+      <c r="C124" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F124" s="13"/>
+      <c r="G124" s="29"/>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F125" s="4"/>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="E127" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F127" s="15" t="s">
+      <c r="G125" s="29"/>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D126" s="2"/>
+      <c r="E126" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F126" s="4"/>
+      <c r="G126" s="29"/>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D127" s="2"/>
+      <c r="E127" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F127" s="4"/>
+      <c r="G127" s="29"/>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D128" s="2"/>
+      <c r="E128" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F128" s="4"/>
+      <c r="G128" s="29"/>
+    </row>
+    <row r="129" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A129" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D129" s="33"/>
+      <c r="E129" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F129" s="34"/>
+      <c r="G129" s="35"/>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="E131" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F131" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
-      <c r="E128" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F128" s="15" t="s">
+    <row r="132" spans="1:7">
+      <c r="E132" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F132" s="15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="5:6">
-      <c r="E129" s="10" t="s">
+    <row r="133" spans="1:7">
+      <c r="E133" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F129" s="15" t="s">
+      <c r="F133" s="15" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B125"/>
   <sortState ref="D378:D392">
     <sortCondition ref="D378"/>
   </sortState>

</xml_diff>

<commit_message>
updates list of supported fUML features
</commit_message>
<xml_diff>
--- a/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
+++ b/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
@@ -436,7 +436,7 @@
     <t>no difference between mode iterative and mode parallel implemented</t>
   </si>
   <si>
-    <t>only support primitive behaviors</t>
+    <t>defining an activity as reducer behavior is not supported</t>
   </si>
 </sst>
 </file>
@@ -1011,9 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -1358,23 +1356,23 @@
       <c r="G20" s="43"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="16" t="s">
+      <c r="A21" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="37" t="s">
+      <c r="D21" s="40"/>
+      <c r="E21" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="42" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds support for structured activity nodes containing call actions
</commit_message>
<xml_diff>
--- a/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
+++ b/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="136">
   <si>
     <t>Actions</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Class</t>
   </si>
   <si>
-    <t>implemented?</t>
-  </si>
-  <si>
     <t>PackageableElement</t>
   </si>
   <si>
@@ -394,39 +391,21 @@
     <t>abstract?</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
-    <t>nt</t>
-  </si>
-  <si>
-    <t>not tested but should work</t>
-  </si>
-  <si>
     <t>Activity Diagrams</t>
   </si>
   <si>
     <t>Class Diagrams</t>
   </si>
   <si>
-    <t>partly</t>
-  </si>
-  <si>
     <t>defining an activity as decision node input behavior is not supported</t>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
     <t>actions with isLocallyReentrant = true are not supported</t>
   </si>
   <si>
@@ -437,6 +416,15 @@
   </si>
   <si>
     <t>defining an activity as reducer behavior is not supported</t>
+  </si>
+  <si>
+    <t>restrictions</t>
+  </si>
+  <si>
+    <t>restricted</t>
+  </si>
+  <si>
+    <t>implemenoted?</t>
   </si>
 </sst>
 </file>
@@ -460,7 +448,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,12 +467,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -633,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -692,13 +674,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1036,13 +1011,13 @@
         <v>15</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1">
@@ -1051,7 +1026,7 @@
     </row>
     <row r="3" spans="1:7" s="6" customFormat="1">
       <c r="A3" s="19" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -1094,24 +1069,24 @@
       <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>136</v>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1122,14 +1097,14 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G8" s="29"/>
     </row>
@@ -1141,14 +1116,14 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" s="29"/>
     </row>
@@ -1160,14 +1135,14 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" s="29"/>
     </row>
@@ -1179,14 +1154,14 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G11" s="29"/>
     </row>
@@ -1198,14 +1173,14 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" s="29"/>
     </row>
@@ -1217,14 +1192,14 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G13" s="29"/>
     </row>
@@ -1236,14 +1211,14 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G14" s="29"/>
     </row>
@@ -1255,14 +1230,14 @@
         <v>1</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G15" s="37"/>
     </row>
@@ -1287,35 +1262,35 @@
         <v>2</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="45" t="s">
+      <c r="A18" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" s="48"/>
+      <c r="C18" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" s="43"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="28" t="s">
@@ -1325,14 +1300,14 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G19" s="29"/>
     </row>
@@ -1344,36 +1319,36 @@
         <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" s="43"/>
+        <v>124</v>
+      </c>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>139</v>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1384,14 +1359,14 @@
         <v>2</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G22" s="37"/>
     </row>
@@ -1403,14 +1378,14 @@
         <v>2</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G23" s="37"/>
     </row>
@@ -1435,14 +1410,14 @@
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G25" s="29"/>
     </row>
@@ -1454,14 +1429,14 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G26" s="29"/>
     </row>
@@ -1473,14 +1448,14 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G27" s="29"/>
     </row>
@@ -1492,14 +1467,14 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G28" s="29"/>
     </row>
@@ -1511,14 +1486,14 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" s="29"/>
     </row>
@@ -1530,14 +1505,14 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G30" s="29"/>
     </row>
@@ -1549,14 +1524,14 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G31" s="29"/>
     </row>
@@ -1568,14 +1543,14 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G32" s="29"/>
     </row>
@@ -1587,14 +1562,14 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G33" s="29"/>
     </row>
@@ -1606,14 +1581,14 @@
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" s="29"/>
     </row>
@@ -1625,14 +1600,14 @@
         <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G35" s="29"/>
     </row>
@@ -1644,14 +1619,14 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G36" s="29"/>
     </row>
@@ -1663,14 +1638,14 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G37" s="29"/>
     </row>
@@ -1682,14 +1657,14 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G38" s="29"/>
     </row>
@@ -1701,14 +1676,14 @@
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G39" s="29"/>
     </row>
@@ -1720,14 +1695,14 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G40" s="29"/>
     </row>
@@ -1739,14 +1714,14 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G41" s="29"/>
     </row>
@@ -1758,14 +1733,14 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G42" s="29"/>
     </row>
@@ -1777,14 +1752,14 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G43" s="29"/>
     </row>
@@ -1796,14 +1771,14 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G44" s="29"/>
     </row>
@@ -1839,14 +1814,14 @@
         <v>5</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G47" s="37"/>
     </row>
@@ -1858,14 +1833,14 @@
         <v>5</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G48" s="37"/>
     </row>
@@ -1877,14 +1852,14 @@
         <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G49" s="29"/>
     </row>
@@ -1896,36 +1871,36 @@
         <v>5</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G50" s="37"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="G51" s="42" t="s">
-        <v>137</v>
+      <c r="C51" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G51" s="38" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="11" customFormat="1">
@@ -1949,14 +1924,14 @@
         <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G53" s="29"/>
     </row>
@@ -1968,36 +1943,36 @@
         <v>6</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G54" s="29"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" s="40"/>
-      <c r="E55" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F55" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="G55" s="42" t="s">
-        <v>138</v>
+      <c r="C55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G55" s="38" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="11" customFormat="1">
@@ -2021,14 +1996,14 @@
         <v>7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G57" s="29"/>
     </row>
@@ -2040,14 +2015,14 @@
         <v>7</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G58" s="29"/>
     </row>
@@ -2059,14 +2034,14 @@
         <v>7</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G59" s="29"/>
     </row>
@@ -2078,14 +2053,14 @@
         <v>7</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G60" s="29"/>
     </row>
@@ -2097,14 +2072,14 @@
         <v>7</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G61" s="29"/>
     </row>
@@ -2116,14 +2091,14 @@
         <v>7</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G62" s="29"/>
     </row>
@@ -2135,36 +2110,36 @@
         <v>7</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G63" s="29"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="38" t="s">
+      <c r="A64" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="39" t="s">
+      <c r="B64" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D64" s="40"/>
-      <c r="E64" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F64" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="G64" s="42" t="s">
+      <c r="C64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F64" s="13" t="s">
         <v>134</v>
+      </c>
+      <c r="G64" s="38" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2175,14 +2150,14 @@
         <v>7</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G65" s="29"/>
     </row>
@@ -2194,14 +2169,14 @@
         <v>7</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G66" s="29"/>
     </row>
@@ -2213,14 +2188,14 @@
         <v>7</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G67" s="29"/>
     </row>
@@ -2232,14 +2207,14 @@
         <v>7</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G68" s="29"/>
     </row>
@@ -2251,14 +2226,14 @@
         <v>7</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G69" s="29"/>
     </row>
@@ -2270,14 +2245,14 @@
         <v>7</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G70" s="29"/>
     </row>
@@ -2289,14 +2264,14 @@
         <v>7</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D71" s="33"/>
       <c r="E71" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F71" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G71" s="35"/>
     </row>
@@ -2305,7 +2280,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="19"/>
@@ -2355,11 +2330,11 @@
         <v>9</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="29"/>
@@ -2372,11 +2347,11 @@
         <v>9</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F78" s="14"/>
       <c r="G78" s="29"/>
@@ -2389,11 +2364,11 @@
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F79" s="13"/>
       <c r="G79" s="29"/>
@@ -2410,7 +2385,7 @@
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F80" s="14"/>
       <c r="G80" s="29"/>
@@ -2423,11 +2398,11 @@
         <v>9</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F81" s="13"/>
       <c r="G81" s="29"/>
@@ -2440,11 +2415,11 @@
         <v>9</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F82" s="13"/>
       <c r="G82" s="29"/>
@@ -2457,11 +2432,11 @@
         <v>9</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F83" s="13"/>
       <c r="G83" s="29"/>
@@ -2474,11 +2449,11 @@
         <v>9</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F84" s="13"/>
       <c r="G84" s="29"/>
@@ -2491,11 +2466,11 @@
         <v>9</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F85" s="13"/>
       <c r="G85" s="29"/>
@@ -2508,11 +2483,11 @@
         <v>9</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F86" s="13"/>
       <c r="G86" s="29"/>
@@ -2525,11 +2500,11 @@
         <v>9</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F87" s="13"/>
       <c r="G87" s="29"/>
@@ -2542,11 +2517,11 @@
         <v>9</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F88" s="14"/>
       <c r="G88" s="29"/>
@@ -2559,11 +2534,11 @@
         <v>9</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F89" s="13"/>
       <c r="G89" s="29"/>
@@ -2576,11 +2551,11 @@
         <v>9</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F90" s="13"/>
       <c r="G90" s="29"/>
@@ -2593,11 +2568,11 @@
         <v>9</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F91" s="13"/>
       <c r="G91" s="29"/>
@@ -2610,11 +2585,11 @@
         <v>9</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F92" s="14"/>
       <c r="G92" s="29"/>
@@ -2627,11 +2602,11 @@
         <v>9</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="29"/>
@@ -2644,11 +2619,11 @@
         <v>9</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F94" s="14"/>
       <c r="G94" s="29"/>
@@ -2661,11 +2636,11 @@
         <v>9</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F95" s="13"/>
       <c r="G95" s="29"/>
@@ -2678,11 +2653,11 @@
         <v>9</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F96" s="13"/>
       <c r="G96" s="29"/>
@@ -2695,11 +2670,11 @@
         <v>9</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F97" s="14"/>
       <c r="G97" s="29"/>
@@ -2712,11 +2687,11 @@
         <v>9</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F98" s="13"/>
       <c r="G98" s="29"/>
@@ -2729,11 +2704,11 @@
         <v>9</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F99" s="13"/>
       <c r="G99" s="29"/>
@@ -2746,11 +2721,11 @@
         <v>9</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F100" s="13"/>
       <c r="G100" s="29"/>
@@ -2763,11 +2738,11 @@
         <v>9</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F101" s="13"/>
       <c r="G101" s="29"/>
@@ -2784,7 +2759,7 @@
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F102" s="13"/>
       <c r="G102" s="29"/>
@@ -2797,11 +2772,11 @@
         <v>9</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F103" s="13"/>
       <c r="G103" s="29"/>
@@ -2814,11 +2789,11 @@
         <v>9</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F104" s="13"/>
       <c r="G104" s="29"/>
@@ -2831,11 +2806,11 @@
         <v>9</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F105" s="13"/>
       <c r="G105" s="29"/>
@@ -2848,11 +2823,11 @@
         <v>9</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F106" s="13"/>
       <c r="G106" s="29"/>
@@ -2865,11 +2840,11 @@
         <v>9</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F107" s="13"/>
       <c r="G107" s="29"/>
@@ -2882,11 +2857,11 @@
         <v>9</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D108" s="2"/>
       <c r="E108" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F108" s="14"/>
       <c r="G108" s="29"/>
@@ -2899,11 +2874,11 @@
         <v>9</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F109" s="13"/>
       <c r="G109" s="29"/>
@@ -2916,11 +2891,11 @@
         <v>9</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F110" s="13"/>
       <c r="G110" s="29"/>
@@ -2933,11 +2908,11 @@
         <v>9</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F111" s="14"/>
       <c r="G111" s="29"/>
@@ -2950,11 +2925,11 @@
         <v>9</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F112" s="14"/>
       <c r="G112" s="29"/>
@@ -2967,11 +2942,11 @@
         <v>9</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F113" s="13"/>
       <c r="G113" s="29"/>
@@ -2984,11 +2959,11 @@
         <v>9</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F114" s="13"/>
       <c r="G114" s="29"/>
@@ -3001,11 +2976,11 @@
         <v>9</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D115" s="2"/>
       <c r="E115" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F115" s="14"/>
       <c r="G115" s="29"/>
@@ -3042,11 +3017,11 @@
         <v>11</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D118" s="2"/>
       <c r="E118" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F118" s="13"/>
       <c r="G118" s="29"/>
@@ -3059,11 +3034,11 @@
         <v>11</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D119" s="2"/>
       <c r="E119" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F119" s="13"/>
       <c r="G119" s="29"/>
@@ -3076,11 +3051,11 @@
         <v>11</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F120" s="13"/>
       <c r="G120" s="29"/>
@@ -3093,11 +3068,11 @@
         <v>11</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F121" s="13"/>
       <c r="G121" s="29"/>
@@ -3110,11 +3085,11 @@
         <v>11</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F122" s="13"/>
       <c r="G122" s="29"/>
@@ -3140,11 +3115,11 @@
         <v>12</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F124" s="13"/>
       <c r="G124" s="29"/>
@@ -3157,11 +3132,11 @@
         <v>12</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F125" s="4"/>
       <c r="G125" s="29"/>
@@ -3174,11 +3149,11 @@
         <v>12</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D126" s="2"/>
       <c r="E126" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F126" s="4"/>
       <c r="G126" s="29"/>
@@ -3191,11 +3166,11 @@
         <v>12</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F127" s="4"/>
       <c r="G127" s="29"/>
@@ -3208,11 +3183,11 @@
         <v>12</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D128" s="2"/>
       <c r="E128" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F128" s="4"/>
       <c r="G128" s="29"/>
@@ -3225,38 +3200,23 @@
         <v>12</v>
       </c>
       <c r="C129" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D129" s="33"/>
       <c r="E129" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F129" s="34"/>
       <c r="G129" s="35"/>
     </row>
     <row r="131" spans="1:7">
-      <c r="E131" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F131" s="15" t="s">
-        <v>126</v>
-      </c>
+      <c r="F131" s="15"/>
     </row>
     <row r="132" spans="1:7">
-      <c r="E132" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F132" s="15" t="s">
-        <v>128</v>
-      </c>
+      <c r="F132" s="15"/>
     </row>
     <row r="133" spans="1:7">
-      <c r="E133" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F133" s="15" t="s">
-        <v>130</v>
-      </c>
+      <c r="F133" s="15"/>
     </row>
   </sheetData>
   <sortState ref="D378:D392">

</xml_diff>

<commit_message>
adds support for conditional nodes
</commit_message>
<xml_diff>
--- a/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
+++ b/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
@@ -986,7 +986,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -1807,42 +1809,42 @@
       <c r="G46" s="27"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G47" s="37"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G47" s="38"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="37"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="38"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="28" t="s">

</xml_diff>

<commit_message>
adds support for loop nodes untestes since it is not clear how loop nodes can be used
</commit_message>
<xml_diff>
--- a/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
+++ b/org.modelexecution.fumldebug.core/docu/fUML_concepts.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="137">
   <si>
     <t>Actions</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>implemenoted?</t>
+  </si>
+  <si>
+    <t>loopVariableInput, loopVariable, and bodyOutput are unclear</t>
   </si>
 </sst>
 </file>
@@ -986,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1882,7 +1885,9 @@
       <c r="F50" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="G50" s="37"/>
+      <c r="G50" s="37" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="30" t="s">

</xml_diff>